<commit_message>
collection report function and fixed upload sales error
</commit_message>
<xml_diff>
--- a/uploads/excel/wesm_purchases_adjust0.xlsx
+++ b/uploads/excel/wesm_purchases_adjust0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Billing-pc\cenpri billing\BS WESM\Adjustment Billing Statement\2023\1 Due on Jan 25 2023\EXCEL\EXCEL Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Billing-pc\cenpri billing\BS WESM\Adjustment Billing Statement\2023\2 Due on Feb 25 2023\Excel\PURCHASES\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -199,6 +199,15 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">FOR THE ACCOUNT OF:  CENPRI_SS
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t>ADDRESS: #88 Eloisa Q's Bldg., Corner Rizal -</t>
     </r>
     <r>
@@ -272,7 +281,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>January 15, 2023</t>
+      <t>February 15, 2023</t>
     </r>
   </si>
   <si>
@@ -293,7 +302,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Mar 26 - Apr 25, 2022</t>
+      <t>Dec 26 - Jan 25, 2022</t>
     </r>
   </si>
   <si>
@@ -314,7 +323,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>January 25, 2023</t>
+      <t>February 25, 2023</t>
     </r>
   </si>
   <si>
@@ -526,7 +535,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Additional Compensation due to Secondary Price Cap of CENPRI for the additional intervals for the</t>
+      <t>Additional Compensation due on the Claim of SIPC for Must Run Unit (MRU) for the period December</t>
     </r>
     <r>
       <rPr>
@@ -542,7 +551,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>billing period March 26 - April 25, 2022 (installment 4of4)</t>
+      <t>26, 2021 - January 25, 2022</t>
     </r>
   </si>
   <si>
@@ -573,7 +582,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Billing Month (Period): April 2022 (Mar 26 - Apr 25, 2022)</t>
+      <t>Billing Month (Period): January 2022 (Dec 26 - Jan 25, 2022)</t>
     </r>
   </si>
   <si>
@@ -842,7 +851,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Sales</t>
+      <t>Purchases</t>
     </r>
   </si>
   <si>
@@ -894,7 +903,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Sales</t>
+      <t>Purchases</t>
     </r>
   </si>
   <si>
@@ -966,7 +975,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Sales</t>
+      <t>Purchases</t>
     </r>
   </si>
   <si>
@@ -998,8 +1007,94 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Sales</t>
-    </r>
+      <t>Purchases</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>EWT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>SIPC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>GEN</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>N</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Note: Sales/Purchases Include Net Settlement Surplus (NSS) flowback and other flowback amounts.</t>
+    </r>
+  </si>
+  <si>
+    <t>Item No.</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>TS-WAC-187F79-0000021</t>
+  </si>
+  <si>
+    <t>WESM TRANSACTION ALLOCATION
+CENPRI / CENTRAL NEGROS POWER RELIABILITY, INC.
+Billing Month (Period): January 2022 (Dec 26 - Jan 25, 2022)                                                                                                                                                                                                                                                                                                TS-WAC-187F79-0000021</t>
   </si>
   <si>
     <r>
@@ -1030,7 +1125,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Purchases</t>
+      <t>Sales</t>
     </r>
   </si>
   <si>
@@ -1082,7 +1177,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Purchases</t>
+      <t>Sales</t>
     </r>
   </si>
   <si>
@@ -1154,7 +1249,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Purchases</t>
+      <t>Sales</t>
     </r>
   </si>
   <si>
@@ -1186,112 +1281,26 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Purchases</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>EWT</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>SUWECO2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>SUWECO2SS</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>LOAD</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Y</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Note: Sales/Purchases Include Net Settlement Surplus (NSS) flowback and other flowback amounts.</t>
-    </r>
-  </si>
-  <si>
-    <t>Item No.</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>TS-WAC-190F70-0000001</t>
-  </si>
-  <si>
-    <t>SUWECO2</t>
-  </si>
-  <si>
-    <t>SUWECO2SS</t>
-  </si>
-  <si>
-    <t>LOAD</t>
+      <t>Sales</t>
+    </r>
+  </si>
+  <si>
+    <t>SIPC</t>
+  </si>
+  <si>
+    <t>GEN</t>
   </si>
   <si>
     <t>Y</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>-</t>
   </si>
   <si>
-    <t>WESM TRANSACTION ALLOCATION
-CENPRI / CENTRAL NEGROS POWER RELIABILITY, INC.
-Billing Month (Period): April 2022 (Mar 26 - Apr 25, 2022)                                                                                                                                                                                                                                                                                                           TS-WAC-190F70-0000001</t>
-  </si>
-  <si>
-    <t>AddCom - SPC 4/4</t>
+    <t xml:space="preserve">AddCom - MRU </t>
   </si>
 </sst>
 </file>
@@ -1300,8 +1309,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="###0.00;###0.00"/>
-    <numFmt numFmtId="165" formatCode="###0.00_);\(###0.00\)"/>
+    <numFmt numFmtId="164" formatCode="###0.00_);\(###0.00\)"/>
+    <numFmt numFmtId="165" formatCode="###0.00;###0.00"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="29" x14ac:knownFonts="1">
@@ -1703,13 +1712,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1725,29 +1731,86 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="24" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1773,9 +1836,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1818,6 +1878,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -1827,15 +1896,6 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1863,6 +1923,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1899,20 +1968,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1923,82 +1983,22 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="24" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2306,10 +2306,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA37"/>
+  <dimension ref="A1:AA38"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:Q32"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="V33" sqref="V33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2317,8 +2317,8 @@
     <col min="1" max="1" width="2.1640625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
-    <col min="4" max="4" width="5.83203125" customWidth="1"/>
-    <col min="5" max="5" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="4.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
     <col min="6" max="6" width="6.83203125" customWidth="1"/>
     <col min="7" max="7" width="4.6640625" customWidth="1"/>
     <col min="8" max="8" width="2.1640625" customWidth="1"/>
@@ -2340,34 +2340,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="17"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="35"/>
     </row>
     <row r="2" spans="1:18" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2382,636 +2382,637 @@
       </c>
     </row>
     <row r="6" spans="1:18" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="59" t="s">
+      <c r="A10" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="61"/>
+      <c r="B10" s="80"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="80"/>
+      <c r="G10" s="80"/>
+      <c r="H10" s="80"/>
+      <c r="I10" s="80"/>
+      <c r="J10" s="81"/>
     </row>
     <row r="11" spans="1:18" ht="105.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="17"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="35"/>
     </row>
     <row r="12" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="62" t="s">
+      <c r="A12" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="63"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="98" t="s">
+      <c r="B12" s="83"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="85" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="38"/>
+    </row>
+    <row r="13" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="73" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="74"/>
+      <c r="C13" s="75"/>
+      <c r="D13" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="38"/>
+    </row>
+    <row r="14" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="73" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="74"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="38"/>
+    </row>
+    <row r="15" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="76" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="77"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="38"/>
+    </row>
+    <row r="16" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="61" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="62"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="62"/>
+      <c r="I17" s="62"/>
+      <c r="J17" s="62"/>
+      <c r="K17" s="62"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="62"/>
+      <c r="N17" s="62"/>
+      <c r="O17" s="62"/>
+      <c r="P17" s="62"/>
+      <c r="Q17" s="63"/>
+    </row>
+    <row r="18" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="65"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="67" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="68"/>
+      <c r="L18" s="69"/>
+      <c r="M18" s="70">
+        <v>-47.12</v>
+      </c>
+      <c r="N18" s="71"/>
+      <c r="O18" s="71"/>
+      <c r="P18" s="71"/>
+      <c r="Q18" s="72"/>
+    </row>
+    <row r="19" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="53"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
+      <c r="K19" s="53"/>
+      <c r="L19" s="54"/>
+      <c r="M19" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="N19" s="53"/>
+      <c r="O19" s="53"/>
+      <c r="P19" s="53"/>
+      <c r="Q19" s="54"/>
+    </row>
+    <row r="20" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="53"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="53"/>
+      <c r="L20" s="54"/>
+      <c r="M20" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="N20" s="53"/>
+      <c r="O20" s="53"/>
+      <c r="P20" s="53"/>
+      <c r="Q20" s="54"/>
+    </row>
+    <row r="21" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="53"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="53"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="54"/>
+      <c r="M21" s="55">
+        <v>-47.12</v>
+      </c>
+      <c r="N21" s="56"/>
+      <c r="O21" s="56"/>
+      <c r="P21" s="56"/>
+      <c r="Q21" s="57"/>
+    </row>
+    <row r="22" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="53"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="53"/>
+      <c r="L22" s="54"/>
+      <c r="M22" s="55">
+        <v>-5.65</v>
+      </c>
+      <c r="N22" s="56"/>
+      <c r="O22" s="56"/>
+      <c r="P22" s="56"/>
+      <c r="Q22" s="57"/>
+    </row>
+    <row r="23" spans="1:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="50"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="53"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="58">
+        <v>0.94</v>
+      </c>
+      <c r="N23" s="59"/>
+      <c r="O23" s="59"/>
+      <c r="P23" s="59"/>
+      <c r="Q23" s="60"/>
+    </row>
+    <row r="24" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="50"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="53"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="53"/>
+      <c r="K24" s="53"/>
+      <c r="L24" s="53"/>
+      <c r="M24" s="53"/>
+      <c r="N24" s="53"/>
+      <c r="O24" s="53"/>
+      <c r="P24" s="53"/>
+      <c r="Q24" s="54"/>
+    </row>
+    <row r="25" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="47"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="K26" s="53"/>
+      <c r="L26" s="53"/>
+      <c r="M26" s="53"/>
+      <c r="N26" s="53"/>
+      <c r="O26" s="53"/>
+      <c r="P26" s="53"/>
+      <c r="Q26" s="54"/>
+    </row>
+    <row r="27" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="47"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="47"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="K27" s="53"/>
+      <c r="L27" s="53"/>
+      <c r="M27" s="53"/>
+      <c r="N27" s="53"/>
+      <c r="O27" s="53"/>
+      <c r="P27" s="53"/>
+      <c r="Q27" s="54"/>
+    </row>
+    <row r="28" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="47"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="34"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="33"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="33"/>
+      <c r="O28" s="33"/>
+      <c r="P28" s="33"/>
+      <c r="Q28" s="35"/>
+    </row>
+    <row r="29" spans="1:17" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="33"/>
+      <c r="M29" s="33"/>
+      <c r="N29" s="33"/>
+      <c r="O29" s="33"/>
+      <c r="P29" s="33"/>
+      <c r="Q29" s="35"/>
+    </row>
+    <row r="30" spans="1:17" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="45.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="33"/>
+      <c r="M32" s="33"/>
+      <c r="N32" s="33"/>
+      <c r="O32" s="33"/>
+      <c r="P32" s="33"/>
+      <c r="Q32" s="35"/>
+    </row>
+    <row r="33" spans="1:27" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="1:27" ht="51.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="42"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="42"/>
+      <c r="I34" s="42"/>
+      <c r="J34" s="42"/>
+      <c r="K34" s="42"/>
+      <c r="L34" s="42"/>
+      <c r="M34" s="42"/>
+      <c r="N34" s="42"/>
+      <c r="O34" s="42"/>
+      <c r="P34" s="42"/>
+      <c r="Q34" s="42"/>
+      <c r="R34" s="42"/>
+      <c r="S34" s="42"/>
+      <c r="T34" s="42"/>
+      <c r="U34" s="42"/>
+      <c r="V34" s="33"/>
+      <c r="W34" s="33"/>
+      <c r="X34" s="33"/>
+      <c r="Y34" s="33"/>
+      <c r="Z34" s="33"/>
+      <c r="AA34" s="35"/>
+    </row>
+    <row r="35" spans="1:27" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="4"/>
+      <c r="B35" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="43"/>
+      <c r="E35" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G35" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="H35" s="44"/>
+      <c r="I35" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J35" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="K35" s="44"/>
+      <c r="L35" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="M35" s="44"/>
+      <c r="N35" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="O35" s="9"/>
+      <c r="P35" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="20"/>
-    </row>
-    <row r="13" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="53" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="54"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="20"/>
-    </row>
-    <row r="14" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="53" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="54"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="20"/>
-    </row>
-    <row r="15" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="57"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="20"/>
-    </row>
-    <row r="16" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="45"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="45"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="45"/>
-      <c r="O17" s="45"/>
-      <c r="P17" s="45"/>
-      <c r="Q17" s="46"/>
-    </row>
-    <row r="18" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="47" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="48"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="50" t="s">
-        <v>21</v>
-      </c>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="51"/>
-      <c r="L18" s="52"/>
-      <c r="M18" s="50" t="s">
-        <v>21</v>
-      </c>
-      <c r="N18" s="51"/>
-      <c r="O18" s="51"/>
-      <c r="P18" s="51"/>
-      <c r="Q18" s="52"/>
-    </row>
-    <row r="19" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="36"/>
-      <c r="K19" s="36"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="N19" s="36"/>
-      <c r="O19" s="36"/>
-      <c r="P19" s="36"/>
-      <c r="Q19" s="37"/>
-    </row>
-    <row r="20" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="41">
-        <v>4.67</v>
-      </c>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="42"/>
-      <c r="L20" s="43"/>
-      <c r="M20" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="N20" s="36"/>
-      <c r="O20" s="36"/>
-      <c r="P20" s="36"/>
-      <c r="Q20" s="37"/>
-    </row>
-    <row r="21" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="41">
-        <v>4.67</v>
-      </c>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="42"/>
-      <c r="L21" s="43"/>
-      <c r="M21" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="N21" s="36"/>
-      <c r="O21" s="36"/>
-      <c r="P21" s="36"/>
-      <c r="Q21" s="37"/>
-    </row>
-    <row r="22" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="36"/>
-      <c r="L22" s="37"/>
-      <c r="M22" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="N22" s="36"/>
-      <c r="O22" s="36"/>
-      <c r="P22" s="36"/>
-      <c r="Q22" s="37"/>
-    </row>
-    <row r="23" spans="1:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="38">
-        <v>-0.09</v>
-      </c>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="40"/>
-      <c r="M23" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="N23" s="36"/>
-      <c r="O23" s="36"/>
-      <c r="P23" s="36"/>
-      <c r="Q23" s="37"/>
-    </row>
-    <row r="24" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="36"/>
-      <c r="M24" s="36"/>
-      <c r="N24" s="36"/>
-      <c r="O24" s="36"/>
-      <c r="P24" s="36"/>
-      <c r="Q24" s="37"/>
-    </row>
-    <row r="25" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="K26" s="36"/>
-      <c r="L26" s="36"/>
-      <c r="M26" s="36"/>
-      <c r="N26" s="36"/>
-      <c r="O26" s="36"/>
-      <c r="P26" s="36"/>
-      <c r="Q26" s="37"/>
-    </row>
-    <row r="27" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="K27" s="36"/>
-      <c r="L27" s="36"/>
-      <c r="M27" s="36"/>
-      <c r="N27" s="36"/>
-      <c r="O27" s="36"/>
-      <c r="P27" s="36"/>
-      <c r="Q27" s="37"/>
-    </row>
-    <row r="28" spans="1:17" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="17"/>
-    </row>
-    <row r="29" spans="1:17" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
-      <c r="P29" s="15"/>
-      <c r="Q29" s="17"/>
-    </row>
-    <row r="30" spans="1:17" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" ht="45.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15"/>
-      <c r="P32" s="15"/>
-      <c r="Q32" s="17"/>
-    </row>
-    <row r="33" spans="1:27" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="97" t="s">
-        <v>36</v>
-      </c>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="25"/>
-      <c r="L33" s="25"/>
-      <c r="M33" s="25"/>
-      <c r="N33" s="25"/>
-      <c r="O33" s="25"/>
-      <c r="P33" s="25"/>
-      <c r="Q33" s="25"/>
-      <c r="R33" s="25"/>
-      <c r="S33" s="25"/>
-      <c r="T33" s="25"/>
-      <c r="U33" s="25"/>
-      <c r="V33" s="15"/>
-      <c r="W33" s="15"/>
-      <c r="X33" s="15"/>
-      <c r="Y33" s="15"/>
-      <c r="Z33" s="15"/>
-      <c r="AA33" s="17"/>
-    </row>
-    <row r="34" spans="1:27" ht="51.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="5"/>
-      <c r="B34" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C34" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="26"/>
-      <c r="E34" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G34" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="H34" s="27"/>
-      <c r="I34" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J34" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="K34" s="27"/>
-      <c r="L34" s="27" t="s">
+      <c r="Q35" s="44"/>
+      <c r="R35" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="S35" s="44"/>
+      <c r="T35" s="44"/>
+      <c r="U35" s="9"/>
+      <c r="V35" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="M34" s="27"/>
-      <c r="N34" s="7" t="s">
+      <c r="W35" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="O34" s="7"/>
-      <c r="P34" s="27" t="s">
+      <c r="X35" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="Q34" s="27"/>
-      <c r="R34" s="27" t="s">
+      <c r="Y35" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="S34" s="27"/>
-      <c r="T34" s="27"/>
-      <c r="U34" s="7"/>
-      <c r="V34" s="7" t="s">
+      <c r="Z35" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="W34" s="7" t="s">
+      <c r="AA35" s="45"/>
+    </row>
+    <row r="36" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="4"/>
+      <c r="B36" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="X34" s="7" t="s">
+      <c r="C36" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36" s="39"/>
+      <c r="E36" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="Y34" s="7" t="s">
+      <c r="F36" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="Z34" s="26" t="s">
+      <c r="G36" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="AA34" s="28"/>
-    </row>
-    <row r="35" spans="1:27" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="5"/>
-      <c r="B35" s="8" t="s">
+      <c r="H36" s="39"/>
+      <c r="I36" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J36" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="K36" s="40"/>
+      <c r="L36" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="M36" s="39"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="P36" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q36" s="40"/>
+      <c r="R36" s="33"/>
+      <c r="S36" s="33"/>
+      <c r="T36" s="33"/>
+      <c r="U36" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="V36" s="7">
+        <v>-47.12</v>
+      </c>
+      <c r="W36" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="X36" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y36" s="7">
+        <v>-5.65</v>
+      </c>
+      <c r="Z36" s="11"/>
+      <c r="AA36" s="8">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="4"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="33"/>
+      <c r="H37" s="33"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="33"/>
+      <c r="K37" s="33"/>
+      <c r="L37" s="33"/>
+      <c r="M37" s="33"/>
+      <c r="N37" s="33"/>
+      <c r="O37" s="33"/>
+      <c r="P37" s="33"/>
+      <c r="Q37" s="33"/>
+      <c r="R37" s="33"/>
+      <c r="S37" s="33"/>
+      <c r="T37" s="33"/>
+      <c r="U37" s="33"/>
+      <c r="V37" s="33"/>
+      <c r="W37" s="33"/>
+      <c r="X37" s="33"/>
+      <c r="Y37" s="33"/>
+      <c r="Z37" s="33"/>
+      <c r="AA37" s="35"/>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A38" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="D35" s="21"/>
-      <c r="E35" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G35" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="H35" s="21"/>
-      <c r="I35" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="J35" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="K35" s="22"/>
-      <c r="L35" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="M35" s="21"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="P35" s="23">
-        <v>4.67</v>
-      </c>
-      <c r="Q35" s="23"/>
-      <c r="R35" s="15"/>
-      <c r="S35" s="15"/>
-      <c r="T35" s="15"/>
-      <c r="U35" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="V35" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="W35" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="X35" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y35" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z35" s="1"/>
-      <c r="AA35" s="10">
-        <v>-0.09</v>
-      </c>
-    </row>
-    <row r="36" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="5"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="15"/>
-      <c r="P36" s="15"/>
-      <c r="Q36" s="15"/>
-      <c r="R36" s="15"/>
-      <c r="S36" s="15"/>
-      <c r="T36" s="15"/>
-      <c r="U36" s="15"/>
-      <c r="V36" s="15"/>
-      <c r="W36" s="15"/>
-      <c r="X36" s="15"/>
-      <c r="Y36" s="15"/>
-      <c r="Z36" s="15"/>
-      <c r="AA36" s="17"/>
-    </row>
-    <row r="37" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="19"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
-      <c r="L37" s="19"/>
-      <c r="M37" s="19"/>
-      <c r="N37" s="19"/>
-      <c r="O37" s="19"/>
-      <c r="P37" s="19"/>
-      <c r="Q37" s="19"/>
-      <c r="R37" s="19"/>
-      <c r="S37" s="19"/>
-      <c r="T37" s="19"/>
-      <c r="U37" s="19"/>
-      <c r="V37" s="19"/>
-      <c r="W37" s="19"/>
-      <c r="X37" s="19"/>
-      <c r="Y37" s="19"/>
-      <c r="Z37" s="19"/>
-      <c r="AA37" s="20"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="37"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="37"/>
+      <c r="L38" s="37"/>
+      <c r="M38" s="37"/>
+      <c r="N38" s="37"/>
+      <c r="O38" s="37"/>
+      <c r="P38" s="37"/>
+      <c r="Q38" s="37"/>
+      <c r="R38" s="37"/>
+      <c r="S38" s="37"/>
+      <c r="T38" s="37"/>
+      <c r="U38" s="37"/>
+      <c r="V38" s="37"/>
+      <c r="W38" s="37"/>
+      <c r="X38" s="37"/>
+      <c r="Y38" s="37"/>
+      <c r="Z38" s="37"/>
+      <c r="AA38" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="58">
@@ -3056,23 +3057,23 @@
     <mergeCell ref="A29:I29"/>
     <mergeCell ref="J29:Q29"/>
     <mergeCell ref="A32:Q32"/>
-    <mergeCell ref="A33:U33"/>
-    <mergeCell ref="V33:AA33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="P34:Q34"/>
-    <mergeCell ref="R34:T34"/>
-    <mergeCell ref="Z34:AA34"/>
-    <mergeCell ref="R35:T35"/>
-    <mergeCell ref="B36:AA36"/>
-    <mergeCell ref="A37:AA37"/>
+    <mergeCell ref="A34:U34"/>
+    <mergeCell ref="V34:AA34"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="G35:H35"/>
     <mergeCell ref="J35:K35"/>
     <mergeCell ref="L35:M35"/>
     <mergeCell ref="P35:Q35"/>
+    <mergeCell ref="R35:T35"/>
+    <mergeCell ref="Z35:AA35"/>
+    <mergeCell ref="R36:T36"/>
+    <mergeCell ref="B37:AA37"/>
+    <mergeCell ref="A38:AA38"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="P36:Q36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3087,138 +3088,140 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="12.1640625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="86" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="12"/>
-    </row>
-    <row r="2" spans="1:13" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="35"/>
+    </row>
+    <row r="2" spans="1:13" ht="67.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="66" t="s">
+      <c r="F2" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="66" t="s">
+      <c r="H2" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="66" t="s">
+      <c r="I2" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="K2" s="66" t="s">
+      <c r="K2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="L2" s="66" t="s">
+      <c r="L2" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="M2" s="65" t="s">
+      <c r="M2" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="8" t="s">
+      <c r="G3" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="7">
+        <v>-47.12</v>
+      </c>
+      <c r="J3" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="67" t="s">
+      <c r="K3" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="L3" s="7">
+        <v>-5.65</v>
+      </c>
+      <c r="M3" s="8">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="35"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="67" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3" s="67" t="s">
-        <v>56</v>
-      </c>
-      <c r="I3" s="67" t="s">
-        <v>57</v>
-      </c>
-      <c r="J3" s="11"/>
-      <c r="K3" s="68">
-        <v>4.67</v>
-      </c>
-      <c r="L3" s="69"/>
-      <c r="M3" s="10">
-        <v>-0.09</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="17"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="20"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B4:M4"/>
     <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="I1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3232,194 +3235,198 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.5" style="73" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="12.33203125" style="73" customWidth="1"/>
-    <col min="6" max="8" width="9.33203125" style="73"/>
-    <col min="9" max="12" width="12.1640625" style="73" customWidth="1"/>
-    <col min="13" max="16384" width="9.33203125" style="73"/>
+    <col min="1" max="1" width="23.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="12.33203125" style="15" customWidth="1"/>
+    <col min="6" max="8" width="9.33203125" style="15"/>
+    <col min="9" max="12" width="12.1640625" style="15" customWidth="1"/>
+    <col min="13" max="16384" width="9.33203125" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="87" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="88"/>
+      <c r="J1" s="88"/>
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="89"/>
+    </row>
+    <row r="2" spans="1:14" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="16">
+        <v>44972</v>
+      </c>
+      <c r="C2" s="16">
+        <v>44556</v>
+      </c>
+      <c r="D2" s="16">
+        <v>44586</v>
+      </c>
+      <c r="E2" s="16">
+        <v>44982</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="19"/>
+    </row>
+    <row r="3" spans="1:14" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="N3" s="24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="25">
+        <v>1</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" s="27">
+        <v>-47.12</v>
+      </c>
+      <c r="J4" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="72"/>
-    </row>
-    <row r="2" spans="1:14" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="73" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="74">
-        <v>44941</v>
-      </c>
-      <c r="C2" s="74">
-        <v>44646</v>
-      </c>
-      <c r="D2" s="74">
-        <v>44676</v>
-      </c>
-      <c r="E2" s="74">
-        <v>44951</v>
-      </c>
-      <c r="F2" s="75" t="s">
-        <v>68</v>
-      </c>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="77"/>
-    </row>
-    <row r="3" spans="1:14" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="78" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="79" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="80" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="81" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="81" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="81" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="81" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" s="81" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" s="81" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" s="81" t="s">
-        <v>49</v>
-      </c>
-      <c r="K3" s="81" t="s">
-        <v>50</v>
-      </c>
-      <c r="L3" s="81" t="s">
-        <v>51</v>
-      </c>
-      <c r="M3" s="80" t="s">
-        <v>52</v>
-      </c>
-      <c r="N3" s="82" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="83">
-        <v>1</v>
-      </c>
-      <c r="B4" s="83" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="84" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="84" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="84" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="84" t="s">
-        <v>65</v>
-      </c>
-      <c r="G4" s="84" t="s">
-        <v>65</v>
-      </c>
-      <c r="H4" s="84" t="s">
-        <v>65</v>
-      </c>
-      <c r="I4" s="85" t="s">
-        <v>66</v>
-      </c>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86">
-        <v>4.67</v>
-      </c>
-      <c r="L4" s="85"/>
-      <c r="M4" s="85">
-        <v>-0.09</v>
-      </c>
-      <c r="N4" s="87">
+      <c r="K4" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="L4" s="27">
+        <v>-5.65</v>
+      </c>
+      <c r="M4" s="27">
+        <v>0.94</v>
+      </c>
+      <c r="N4" s="29">
         <f>SUM(I4:M4)</f>
-        <v>4.58</v>
+        <v>-51.83</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="88"/>
-      <c r="B5" s="89"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="90"/>
-      <c r="I5" s="90"/>
-      <c r="J5" s="90"/>
-      <c r="K5" s="90"/>
-      <c r="L5" s="90"/>
-      <c r="M5" s="90"/>
-      <c r="N5" s="91"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="90"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
+      <c r="H5" s="91"/>
+      <c r="I5" s="91"/>
+      <c r="J5" s="91"/>
+      <c r="K5" s="91"/>
+      <c r="L5" s="91"/>
+      <c r="M5" s="91"/>
+      <c r="N5" s="92"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="92" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="93"/>
-      <c r="C6" s="93"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="93"/>
-      <c r="K6" s="93"/>
-      <c r="L6" s="93"/>
-      <c r="M6" s="93"/>
-      <c r="N6" s="94"/>
+      <c r="A6" s="93" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="94"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="94"/>
+      <c r="E6" s="94"/>
+      <c r="F6" s="94"/>
+      <c r="G6" s="94"/>
+      <c r="H6" s="94"/>
+      <c r="I6" s="94"/>
+      <c r="J6" s="94"/>
+      <c r="K6" s="94"/>
+      <c r="L6" s="94"/>
+      <c r="M6" s="94"/>
+      <c r="N6" s="95"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="95"/>
+      <c r="A10" s="31"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="95"/>
+      <c r="A12" s="31"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B16" s="95"/>
-      <c r="E16" s="95"/>
+      <c r="B16" s="31"/>
+      <c r="E16" s="31"/>
     </row>
     <row r="18" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="96"/>
+      <c r="A18" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Add checker if there is non numeric value in vatable sales, zeo rated exozone etc. purchases and sales
</commit_message>
<xml_diff>
--- a/uploads/excel/wesm_purchases_adjust0.xlsx
+++ b/uploads/excel/wesm_purchases_adjust0.xlsx
@@ -3831,7 +3831,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4352,6 +4352,6 @@
     <mergeCell ref="A14:N14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>